<commit_message>
finally connected everything (still need UI change/more testing)
</commit_message>
<xml_diff>
--- a/ScanReport.xlsx
+++ b/ScanReport.xlsx
@@ -107,7 +107,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>subject_id</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -136,16 +136,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>drug</t>
+          <t>entry_date</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>varchar</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="E3" t="n">
         <v>2.0</v>
@@ -165,16 +165,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>treatment</t>
+          <t>discharge_date</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>varchar</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n">
         <v>2.0</v>
@@ -183,7 +183,7 @@
         <v>2.0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -194,7 +194,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>drug</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -217,6 +217,64 @@
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
+        <is>
+          <t>new_table</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>effect</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>new_table</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>unique_id</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -238,7 +296,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>subject_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -248,30 +306,50 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>entry_date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>discharge_date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>drug</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Frequency</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>treatment</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Frequency</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>effect</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>unique_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -314,6 +392,26 @@
         </is>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>List truncated...</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>List truncated...</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>